<commit_message>
update energy demand baseline input data
</commit_message>
<xml_diff>
--- a/data/weo_gcam_dict.xlsx
+++ b/data/weo_gcam_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/PD21/positive-disruption/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E53E21-56C9-9B4C-BA79-8D2D72F783D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9539AD-A78A-7747-ADB3-CB2141B84162}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{CEDCD615-163B-E44B-8233-987F67EF32ED}"/>
   </bookViews>
@@ -228,7 +228,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="69">
   <si>
     <t>TFC</t>
   </si>
@@ -773,86 +773,86 @@
       <sheetName val="Data Sources"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
-      <sheetData sheetId="49" refreshError="1"/>
-      <sheetData sheetId="50" refreshError="1"/>
-      <sheetData sheetId="51" refreshError="1"/>
-      <sheetData sheetId="52" refreshError="1"/>
-      <sheetData sheetId="53" refreshError="1"/>
-      <sheetData sheetId="54" refreshError="1"/>
-      <sheetData sheetId="55" refreshError="1"/>
-      <sheetData sheetId="56" refreshError="1"/>
-      <sheetData sheetId="57" refreshError="1"/>
-      <sheetData sheetId="58" refreshError="1"/>
-      <sheetData sheetId="59" refreshError="1"/>
-      <sheetData sheetId="60" refreshError="1"/>
-      <sheetData sheetId="61" refreshError="1"/>
-      <sheetData sheetId="62" refreshError="1"/>
-      <sheetData sheetId="63" refreshError="1"/>
-      <sheetData sheetId="64" refreshError="1"/>
-      <sheetData sheetId="65" refreshError="1"/>
-      <sheetData sheetId="66" refreshError="1"/>
-      <sheetData sheetId="67" refreshError="1"/>
-      <sheetData sheetId="68" refreshError="1"/>
-      <sheetData sheetId="69" refreshError="1"/>
-      <sheetData sheetId="70" refreshError="1"/>
-      <sheetData sheetId="71" refreshError="1"/>
-      <sheetData sheetId="72" refreshError="1"/>
-      <sheetData sheetId="73" refreshError="1"/>
-      <sheetData sheetId="74" refreshError="1"/>
-      <sheetData sheetId="75" refreshError="1"/>
-      <sheetData sheetId="76" refreshError="1"/>
-      <sheetData sheetId="77" refreshError="1"/>
-      <sheetData sheetId="78" refreshError="1"/>
-      <sheetData sheetId="79" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50"/>
+      <sheetData sheetId="51"/>
+      <sheetData sheetId="52"/>
+      <sheetData sheetId="53"/>
+      <sheetData sheetId="54"/>
+      <sheetData sheetId="55"/>
+      <sheetData sheetId="56"/>
+      <sheetData sheetId="57"/>
+      <sheetData sheetId="58"/>
+      <sheetData sheetId="59"/>
+      <sheetData sheetId="60"/>
+      <sheetData sheetId="61"/>
+      <sheetData sheetId="62"/>
+      <sheetData sheetId="63"/>
+      <sheetData sheetId="64"/>
+      <sheetData sheetId="65"/>
+      <sheetData sheetId="66"/>
+      <sheetData sheetId="67"/>
+      <sheetData sheetId="68"/>
+      <sheetData sheetId="69"/>
+      <sheetData sheetId="70"/>
+      <sheetData sheetId="71"/>
+      <sheetData sheetId="72"/>
+      <sheetData sheetId="73"/>
+      <sheetData sheetId="74"/>
+      <sheetData sheetId="75"/>
+      <sheetData sheetId="76"/>
+      <sheetData sheetId="77"/>
+      <sheetData sheetId="78"/>
+      <sheetData sheetId="79"/>
       <sheetData sheetId="80">
         <row r="2">
           <cell r="E2">
@@ -860,14 +860,14 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="81" refreshError="1"/>
-      <sheetData sheetId="82" refreshError="1"/>
-      <sheetData sheetId="83" refreshError="1"/>
-      <sheetData sheetId="84" refreshError="1"/>
-      <sheetData sheetId="85" refreshError="1"/>
-      <sheetData sheetId="86" refreshError="1"/>
-      <sheetData sheetId="87" refreshError="1"/>
-      <sheetData sheetId="88" refreshError="1"/>
+      <sheetData sheetId="81"/>
+      <sheetData sheetId="82"/>
+      <sheetData sheetId="83"/>
+      <sheetData sheetId="84"/>
+      <sheetData sheetId="85"/>
+      <sheetData sheetId="86"/>
+      <sheetData sheetId="87"/>
+      <sheetData sheetId="88"/>
       <sheetData sheetId="89">
         <row r="33">
           <cell r="I33">
@@ -875,37 +875,37 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="90" refreshError="1"/>
-      <sheetData sheetId="91" refreshError="1"/>
-      <sheetData sheetId="92" refreshError="1"/>
-      <sheetData sheetId="93" refreshError="1"/>
-      <sheetData sheetId="94" refreshError="1"/>
-      <sheetData sheetId="95" refreshError="1"/>
-      <sheetData sheetId="96" refreshError="1"/>
-      <sheetData sheetId="97" refreshError="1"/>
-      <sheetData sheetId="98" refreshError="1"/>
-      <sheetData sheetId="99" refreshError="1"/>
-      <sheetData sheetId="100" refreshError="1"/>
-      <sheetData sheetId="101" refreshError="1"/>
-      <sheetData sheetId="102" refreshError="1"/>
-      <sheetData sheetId="103" refreshError="1"/>
-      <sheetData sheetId="104" refreshError="1"/>
-      <sheetData sheetId="105" refreshError="1"/>
-      <sheetData sheetId="106" refreshError="1"/>
-      <sheetData sheetId="107" refreshError="1"/>
-      <sheetData sheetId="108" refreshError="1"/>
-      <sheetData sheetId="109" refreshError="1"/>
-      <sheetData sheetId="110" refreshError="1"/>
-      <sheetData sheetId="111" refreshError="1"/>
-      <sheetData sheetId="112" refreshError="1"/>
-      <sheetData sheetId="113" refreshError="1"/>
-      <sheetData sheetId="114" refreshError="1"/>
-      <sheetData sheetId="115" refreshError="1"/>
-      <sheetData sheetId="116" refreshError="1"/>
-      <sheetData sheetId="117" refreshError="1"/>
-      <sheetData sheetId="118" refreshError="1"/>
-      <sheetData sheetId="119" refreshError="1"/>
-      <sheetData sheetId="120" refreshError="1"/>
+      <sheetData sheetId="90"/>
+      <sheetData sheetId="91"/>
+      <sheetData sheetId="92"/>
+      <sheetData sheetId="93"/>
+      <sheetData sheetId="94"/>
+      <sheetData sheetId="95"/>
+      <sheetData sheetId="96"/>
+      <sheetData sheetId="97"/>
+      <sheetData sheetId="98"/>
+      <sheetData sheetId="99"/>
+      <sheetData sheetId="100"/>
+      <sheetData sheetId="101"/>
+      <sheetData sheetId="102"/>
+      <sheetData sheetId="103"/>
+      <sheetData sheetId="104"/>
+      <sheetData sheetId="105"/>
+      <sheetData sheetId="106"/>
+      <sheetData sheetId="107"/>
+      <sheetData sheetId="108"/>
+      <sheetData sheetId="109"/>
+      <sheetData sheetId="110"/>
+      <sheetData sheetId="111"/>
+      <sheetData sheetId="112"/>
+      <sheetData sheetId="113"/>
+      <sheetData sheetId="114"/>
+      <sheetData sheetId="115"/>
+      <sheetData sheetId="116"/>
+      <sheetData sheetId="117"/>
+      <sheetData sheetId="118"/>
+      <sheetData sheetId="119"/>
+      <sheetData sheetId="120"/>
       <sheetData sheetId="121">
         <row r="6">
           <cell r="G6">
@@ -954,7 +954,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="125" refreshError="1"/>
+      <sheetData sheetId="125"/>
       <sheetData sheetId="126">
         <row r="4">
           <cell r="C4">
@@ -1111,8 +1111,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="137" refreshError="1"/>
-      <sheetData sheetId="138" refreshError="1"/>
+      <sheetData sheetId="137"/>
+      <sheetData sheetId="138"/>
       <sheetData sheetId="139">
         <row r="6">
           <cell r="G6">
@@ -1428,13 +1428,13 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="143" refreshError="1"/>
-      <sheetData sheetId="144" refreshError="1"/>
-      <sheetData sheetId="145" refreshError="1"/>
-      <sheetData sheetId="146" refreshError="1"/>
-      <sheetData sheetId="147" refreshError="1"/>
-      <sheetData sheetId="148" refreshError="1"/>
-      <sheetData sheetId="149" refreshError="1"/>
+      <sheetData sheetId="143"/>
+      <sheetData sheetId="144"/>
+      <sheetData sheetId="145"/>
+      <sheetData sheetId="146"/>
+      <sheetData sheetId="147"/>
+      <sheetData sheetId="148"/>
+      <sheetData sheetId="149"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2305,8 +2305,8 @@
   </sheetPr>
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2419,6 +2419,9 @@
       <c r="A10" t="s">
         <v>26</v>
       </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
       <c r="C10" t="s">
         <v>48</v>
       </c>
@@ -2504,6 +2507,9 @@
       <c r="A18" t="s">
         <v>14</v>
       </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
       <c r="C18" t="s">
         <v>61</v>
       </c>
@@ -2611,6 +2617,9 @@
       <c r="A28" t="s">
         <v>3</v>
       </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
       <c r="C28" s="2" t="s">
         <v>36</v>
       </c>
@@ -2696,6 +2705,9 @@
       <c r="A36" t="s">
         <v>5</v>
       </c>
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
       <c r="C36" s="2" t="s">
         <v>13</v>
       </c>
@@ -2759,6 +2771,9 @@
       <c r="A42" t="s">
         <v>7</v>
       </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
       <c r="C42" s="2" t="s">
         <v>63</v>
       </c>
@@ -2853,6 +2868,9 @@
     </row>
     <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" t="s">
         <v>9</v>
       </c>
       <c r="C51" s="2" t="s">

</xml_diff>